<commit_message>
add check plant selection script
</commit_message>
<xml_diff>
--- a/calculations/gewicht beet.xlsx
+++ b/calculations/gewicht beet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/Medieninformatik_Master/4.Sem/AWE Smart Campus/plant_matcher/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/Medieninformatik_Master/4.Sem/AWE Smart Campus/plant-data/calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2C0FEF-8A72-A942-BE5C-4D090F652065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE745C17-BB6D-C548-B176-CDB105C4C639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57600" yWindow="-7500" windowWidth="28800" windowHeight="23500" xr2:uid="{A8072F7E-3992-DD44-8229-9F5F87733D00}"/>
+    <workbookView xWindow="-28800" yWindow="-7500" windowWidth="28800" windowHeight="23500" xr2:uid="{A8072F7E-3992-DD44-8229-9F5F87733D00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Breite</t>
   </si>
@@ -85,9 +86,6 @@
   </si>
   <si>
     <t>maximal mit Wasserzuschlag (*1,4)</t>
-  </si>
-  <si>
-    <t>Materialien</t>
   </si>
   <si>
     <t>Gesamtvolumen Blähton</t>
@@ -470,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8137A2-7231-5944-8DAD-AA470D635EC3}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,8 +534,8 @@
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <f>1/4</f>
-        <v>0.25</v>
+        <f>8/40</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -557,7 +555,7 @@
       </c>
       <c r="B9">
         <f>B7*B4*B8</f>
-        <v>24</v>
+        <v>19.2</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -565,11 +563,11 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <f>B7*B4</f>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -585,8 +583,8 @@
         <v>7</v>
       </c>
       <c r="B13" s="1">
-        <f>3/4</f>
-        <v>0.75</v>
+        <f>32/40</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -606,7 +604,7 @@
       </c>
       <c r="B15">
         <f>B4*B13*B14</f>
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -618,7 +616,7 @@
       </c>
       <c r="B17" s="3">
         <f>B9+B15</f>
-        <v>144</v>
+        <v>147.19999999999999</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
@@ -630,15 +628,10 @@
       </c>
       <c r="B18" s="2">
         <f>B17*1.4</f>
-        <v>201.6</v>
+        <v>206.07999999999998</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>